<commit_message>
Add the TrialInput Data Set to the Import Folder which is used if using the Tool via python scripts, not GUI.
</commit_message>
<xml_diff>
--- a/02_Tool/Data/InputData.xlsx
+++ b/02_Tool/Data/InputData.xlsx
@@ -36,22 +36,22 @@
     <t>FreshAir Temperature [Deg. C]</t>
   </si>
   <si>
-    <t>Space Temperature T1 [Deg. C]_y</t>
-  </si>
-  <si>
-    <t>Space Temperature T2 [Deg. C]_y</t>
-  </si>
-  <si>
     <t>Av. Space Temperature [Deg. C]</t>
-  </si>
-  <si>
-    <t>Supply Temperature [Deg. C]_y</t>
   </si>
   <si>
     <t>Triad Lvl 2[]</t>
   </si>
   <si>
     <t>Load Shed[]</t>
+  </si>
+  <si>
+    <t>Space Temperature T1 [Deg. C]</t>
+  </si>
+  <si>
+    <t>Space Temperature T2 [Deg. C]</t>
+  </si>
+  <si>
+    <t>Supply Temperature [Deg. C]</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:K1537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,22 +401,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>